<commit_message>
no exch risulta meglio
</commit_message>
<xml_diff>
--- a/test_cuda_queue_no_exch/E_20/Test_NOEXCH_E20.xlsx
+++ b/test_cuda_queue_no_exch/E_20/Test_NOEXCH_E20.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\progetto\test_cuda_queue\E_20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\test_cuda_queue_no_exch\E_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="[$€-410]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$€-410]&quot; &quot;#,##0.00"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -297,28 +297,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>18.27257617728532</c:v>
+                  <c:v>20.297391513403053</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.917047184170475</c:v>
+                  <c:v>23.332043664501864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.172165874951855</c:v>
+                  <c:v>24.362141105179628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.188487729667223</c:v>
+                  <c:v>23.910223732653638</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.202131569276002</c:v>
+                  <c:v>24.682648735564975</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.559681004052816</c:v>
+                  <c:v>23.889926428975663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0854-435B-B229-DAC4B5BBD242}"/>
             </c:ext>
@@ -388,28 +388,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>21.057397959183675</c:v>
+                  <c:v>23.719794499848895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.757064364207224</c:v>
+                  <c:v>27.365176765915905</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.264965259219668</c:v>
+                  <c:v>28.731532323010473</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.466950959488273</c:v>
+                  <c:v>27.929969397195929</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.447899838449111</c:v>
+                  <c:v>29.254118524040255</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.625707409093867</c:v>
+                  <c:v>27.264415728775877</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0854-435B-B229-DAC4B5BBD242}"/>
             </c:ext>
@@ -479,28 +479,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>23.867886744173109</c:v>
+                  <c:v>24.937471770551038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.139080109655804</c:v>
+                  <c:v>29.413811474045218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.890662241665407</c:v>
+                  <c:v>29.461879669156882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.54333436436746</c:v>
+                  <c:v>29.248253484753167</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.340464716535188</c:v>
+                  <c:v>29.045340961399354</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.907076440043475</c:v>
+                  <c:v>29.231800132362672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0854-435B-B229-DAC4B5BBD242}"/>
             </c:ext>
@@ -570,28 +570,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>22.198972038325092</c:v>
+                  <c:v>23.087281611986871</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.56659697818899</c:v>
+                  <c:v>25.130541358924653</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.944364245293912</c:v>
+                  <c:v>24.471862957704726</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.856925090239727</c:v>
+                  <c:v>24.279060768349691</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.139442115071045</c:v>
+                  <c:v>24.150841429429242</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.47956214084174</c:v>
+                  <c:v>23.839944677487992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0854-435B-B229-DAC4B5BBD242}"/>
             </c:ext>
@@ -926,7 +926,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -1071,28 +1071,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.081740732212756</c:v>
+                  <c:v>11.083686176836864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.38159604886925</c:v>
+                  <c:v>12.289698978182823</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.424801362088536</c:v>
+                  <c:v>13.345629029839557</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.762256548018804</c:v>
+                  <c:v>13.357646705688129</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.132169576059852</c:v>
+                  <c:v>13.667383292383294</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.757985257985258</c:v>
+                  <c:v>11.518312411026271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0EA3-4CE5-BEDC-F4E348063810}"/>
             </c:ext>
@@ -1162,28 +1162,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>11.183869389751743</c:v>
+                  <c:v>11.671021960495644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.724433004035063</c:v>
+                  <c:v>14.745485545997054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.889808626974485</c:v>
+                  <c:v>15.320154601819793</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.94168762863023</c:v>
+                  <c:v>14.82476235000779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.859286201409411</c:v>
+                  <c:v>15.14937495023489</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.516969964108053</c:v>
+                  <c:v>13.099765904709445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0EA3-4CE5-BEDC-F4E348063810}"/>
             </c:ext>
@@ -1253,28 +1253,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16.966765501287021</c:v>
+                  <c:v>15.595868191907119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.99146577190999</c:v>
+                  <c:v>18.329855118995063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.109171654759606</c:v>
+                  <c:v>19.917360777986129</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.069644646573654</c:v>
+                  <c:v>19.916492237920806</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.543141302308126</c:v>
+                  <c:v>19.663538123735307</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.206152524451493</c:v>
+                  <c:v>15.977226614426641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0EA3-4CE5-BEDC-F4E348063810}"/>
             </c:ext>
@@ -1344,28 +1344,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>20.660844299542209</c:v>
+                  <c:v>18.504486033715349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.886475072474145</c:v>
+                  <c:v>21.860162298679253</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.70771058836635</c:v>
+                  <c:v>22.970503143285985</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.590248042279057</c:v>
+                  <c:v>22.919649252273569</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.884032481383077</c:v>
+                  <c:v>23.005533648504393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.675680893164525</c:v>
+                  <c:v>19.058204591394745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0EA3-4CE5-BEDC-F4E348063810}"/>
             </c:ext>
@@ -3753,7 +3753,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="D56" sqref="D56:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3811,14 +3811,14 @@
         <v>32</v>
       </c>
       <c r="D4">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E4">
-        <v>9.0249999999999997E-2</v>
+        <v>8.319E-2</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F9" si="0">D4/E4</f>
-        <v>18.27257617728532</v>
+        <v>20.297391513403053</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3832,14 +3832,14 @@
         <v>64</v>
       </c>
       <c r="D5">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E5">
-        <v>7.8839999999999993E-2</v>
+        <v>7.2370000000000004E-2</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>20.917047184170475</v>
+        <v>23.332043664501864</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3853,14 +3853,14 @@
         <v>128</v>
       </c>
       <c r="D6">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E6">
-        <v>7.7890000000000001E-2</v>
+        <v>6.9309999999999997E-2</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>21.172165874951855</v>
+        <v>24.362141105179628</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3874,14 +3874,14 @@
         <v>256</v>
       </c>
       <c r="D7">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E7">
-        <v>7.7829999999999996E-2</v>
+        <v>7.0620000000000002E-2</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>21.188487729667223</v>
+        <v>23.910223732653638</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
@@ -3898,14 +3898,14 @@
         <v>512</v>
       </c>
       <c r="D8">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E8">
-        <v>8.1629999999999994E-2</v>
+        <v>6.8409999999999999E-2</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>20.202131569276002</v>
+        <v>24.682648735564975</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3919,14 +3919,14 @@
         <v>1024</v>
       </c>
       <c r="D9">
-        <v>1.6491</v>
+        <v>1.6885399999999999</v>
       </c>
       <c r="E9">
-        <v>7.6490000000000002E-2</v>
+        <v>7.0680000000000007E-2</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>21.559681004052816</v>
+        <v>23.889926428975663</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3943,14 +3943,14 @@
         <v>32</v>
       </c>
       <c r="D11">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E11">
-        <v>0.17247999999999999</v>
+        <v>0.16545000000000001</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" ref="F11:F16" si="1">D11/E11</f>
-        <v>21.057397959183675</v>
+        <v>23.719794499848895</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3964,14 +3964,14 @@
         <v>64</v>
       </c>
       <c r="D12">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E12">
-        <v>0.15287999999999999</v>
+        <v>0.14341000000000001</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>23.757064364207224</v>
+        <v>27.365176765915905</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3985,14 +3985,14 @@
         <v>128</v>
       </c>
       <c r="D13">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E13">
-        <v>0.14968000000000001</v>
+        <v>0.13658999999999999</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>24.264965259219668</v>
+        <v>28.731532323010473</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4006,14 +4006,14 @@
         <v>256</v>
       </c>
       <c r="D14">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E14">
-        <v>0.15476999999999999</v>
+        <v>0.14051</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>23.466950959488273</v>
+        <v>27.929969397195929</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
@@ -4030,14 +4030,14 @@
         <v>512</v>
       </c>
       <c r="D15">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E15">
-        <v>0.14856</v>
+        <v>0.13414999999999999</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>24.447899838449111</v>
+        <v>29.254118524040255</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4051,14 +4051,14 @@
         <v>1024</v>
       </c>
       <c r="D16">
-        <v>3.63198</v>
+        <v>3.9244400000000002</v>
       </c>
       <c r="E16">
-        <v>0.15373000000000001</v>
+        <v>0.14394000000000001</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>23.625707409093867</v>
+        <v>27.264415728775877</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4075,14 +4075,14 @@
         <v>32</v>
       </c>
       <c r="D18">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E18">
-        <v>0.35954000000000003</v>
+        <v>0.35424</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:F23" si="2">D18/E18</f>
-        <v>23.867886744173109</v>
+        <v>24.937471770551038</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4096,14 +4096,14 @@
         <v>64</v>
       </c>
       <c r="D19">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E19">
-        <v>0.32829999999999998</v>
+        <v>0.30032999999999999</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>26.139080109655804</v>
+        <v>29.413811474045218</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -4117,14 +4117,14 @@
         <v>128</v>
       </c>
       <c r="D20">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E20">
-        <v>0.33145000000000002</v>
+        <v>0.29984</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>25.890662241665407</v>
+        <v>29.461879669156882</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4138,14 +4138,14 @@
         <v>256</v>
       </c>
       <c r="D21">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E21">
-        <v>0.32329999999999998</v>
+        <v>0.30203000000000002</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>26.54333436436746</v>
+        <v>29.248253484753167</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>7</v>
@@ -4162,14 +4162,14 @@
         <v>512</v>
       </c>
       <c r="D22">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E22">
-        <v>0.32579000000000002</v>
+        <v>0.30414000000000002</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>26.340464716535188</v>
+        <v>29.045340961399354</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4183,14 +4183,14 @@
         <v>1024</v>
       </c>
       <c r="D23">
-        <v>8.5814599999999999</v>
+        <v>8.83385</v>
       </c>
       <c r="E23">
-        <v>0.33123999999999998</v>
+        <v>0.30220000000000002</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>25.907076440043475</v>
+        <v>29.231800132362672</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -4207,14 +4207,14 @@
         <v>32</v>
       </c>
       <c r="D25">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E25">
-        <v>0.71597999999999995</v>
+        <v>0.67940999999999996</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25:F30" si="3">D25/E25</f>
-        <v>22.198972038325092</v>
+        <v>23.087281611986871</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -4228,14 +4228,14 @@
         <v>64</v>
       </c>
       <c r="D26">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E26">
-        <v>0.67442999999999997</v>
+        <v>0.62417</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="3"/>
-        <v>23.56659697818899</v>
+        <v>25.130541358924653</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -4249,14 +4249,14 @@
         <v>128</v>
       </c>
       <c r="D27">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E27">
-        <v>0.69272</v>
+        <v>0.64097000000000004</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="3"/>
-        <v>22.944364245293912</v>
+        <v>24.471862957704726</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -4270,14 +4270,14 @@
         <v>256</v>
       </c>
       <c r="D28">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E28">
-        <v>0.69537000000000004</v>
+        <v>0.64605999999999997</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="3"/>
-        <v>22.856925090239727</v>
+        <v>24.279060768349691</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>7</v>
@@ -4294,14 +4294,14 @@
         <v>512</v>
       </c>
       <c r="D29">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E29">
-        <v>0.68688000000000005</v>
+        <v>0.64949000000000001</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="3"/>
-        <v>23.139442115071045</v>
+        <v>24.150841429429242</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -4315,14 +4315,14 @@
         <v>1024</v>
       </c>
       <c r="D30">
-        <v>15.894019999999999</v>
+        <v>15.68573</v>
       </c>
       <c r="E30">
-        <v>0.67693000000000003</v>
+        <v>0.65795999999999999</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="3"/>
-        <v>23.47956214084174</v>
+        <v>23.839944677487992</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -4377,14 +4377,14 @@
         <v>32</v>
       </c>
       <c r="D35">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E35">
-        <v>8.6860000000000007E-2</v>
+        <v>8.0299999999999996E-2</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" ref="F35:F40" si="4">D35/E35</f>
-        <v>10.081740732212756</v>
+        <v>11.083686176836864</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -4398,14 +4398,14 @@
         <v>64</v>
       </c>
       <c r="D36">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E36">
-        <v>7.6939999999999995E-2</v>
+        <v>7.2419999999999998E-2</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="4"/>
-        <v>11.38159604886925</v>
+        <v>12.289698978182823</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -4419,14 +4419,14 @@
         <v>128</v>
       </c>
       <c r="D37">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E37">
-        <v>7.0480000000000001E-2</v>
+        <v>6.6689999999999999E-2</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="4"/>
-        <v>12.424801362088536</v>
+        <v>13.345629029839557</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -4440,14 +4440,14 @@
         <v>256</v>
       </c>
       <c r="D38">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E38">
-        <v>7.4450000000000002E-2</v>
+        <v>6.6629999999999995E-2</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="4"/>
-        <v>11.762256548018804</v>
+        <v>13.357646705688129</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>7</v>
@@ -4464,14 +4464,14 @@
         <v>512</v>
       </c>
       <c r="D39">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E39">
-        <v>7.2179999999999994E-2</v>
+        <v>6.5119999999999997E-2</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" si="4"/>
-        <v>12.132169576059852</v>
+        <v>13.667383292383294</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -4485,14 +4485,14 @@
         <v>1024</v>
       </c>
       <c r="D40">
-        <v>0.87570000000000003</v>
+        <v>0.89002000000000003</v>
       </c>
       <c r="E40">
-        <v>8.14E-2</v>
+        <v>7.7270000000000005E-2</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" si="4"/>
-        <v>10.757985257985258</v>
+        <v>11.518312411026271</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -4509,14 +4509,14 @@
         <v>32</v>
       </c>
       <c r="D42">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E42">
-        <v>0.16353999999999999</v>
+        <v>0.16302</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" ref="F42:F47" si="5">D42/E42</f>
-        <v>11.183869389751743</v>
+        <v>11.671021960495644</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -4530,14 +4530,14 @@
         <v>64</v>
       </c>
       <c r="D43">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E43">
-        <v>0.14374000000000001</v>
+        <v>0.12903000000000001</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" si="5"/>
-        <v>12.724433004035063</v>
+        <v>14.745485545997054</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -4551,14 +4551,14 @@
         <v>128</v>
       </c>
       <c r="D44">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E44">
-        <v>0.13167999999999999</v>
+        <v>0.12418999999999999</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" si="5"/>
-        <v>13.889808626974485</v>
+        <v>15.320154601819793</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -4572,14 +4572,14 @@
         <v>256</v>
       </c>
       <c r="D45">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E45">
-        <v>0.13119</v>
+        <v>0.12834000000000001</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" si="5"/>
-        <v>13.94168762863023</v>
+        <v>14.82476235000779</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>7</v>
@@ -4596,14 +4596,14 @@
         <v>512</v>
       </c>
       <c r="D46">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E46">
-        <v>0.13197</v>
+        <v>0.12559000000000001</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" si="5"/>
-        <v>13.859286201409411</v>
+        <v>15.14937495023489</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -4617,14 +4617,14 @@
         <v>1024</v>
       </c>
       <c r="D47">
-        <v>1.82901</v>
+        <v>1.9026099999999999</v>
       </c>
       <c r="E47">
-        <v>0.15881000000000001</v>
+        <v>0.14524000000000001</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" si="5"/>
-        <v>11.516969964108053</v>
+        <v>13.099765904709445</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -4641,14 +4641,14 @@
         <v>32</v>
       </c>
       <c r="D49">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E49">
-        <v>0.30691000000000002</v>
+        <v>0.29285</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" ref="F49:F54" si="6">D49/E49</f>
-        <v>16.966765501287021</v>
+        <v>15.595868191907119</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -4662,14 +4662,14 @@
         <v>64</v>
       </c>
       <c r="D50">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E50">
-        <v>0.27418999999999999</v>
+        <v>0.24917</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" si="6"/>
-        <v>18.99146577190999</v>
+        <v>18.329855118995063</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -4683,14 +4683,14 @@
         <v>128</v>
       </c>
       <c r="D51">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E51">
-        <v>0.25895000000000001</v>
+        <v>0.22931000000000001</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" si="6"/>
-        <v>20.109171654759606</v>
+        <v>19.917360777986129</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -4704,14 +4704,14 @@
         <v>256</v>
       </c>
       <c r="D52">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E52">
-        <v>0.25946000000000002</v>
+        <v>0.22932</v>
       </c>
       <c r="F52" s="2">
         <f t="shared" si="6"/>
-        <v>20.069644646573654</v>
+        <v>19.916492237920806</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>7</v>
@@ -4728,14 +4728,14 @@
         <v>512</v>
       </c>
       <c r="D53">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E53">
-        <v>0.26645000000000002</v>
+        <v>0.23227</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" si="6"/>
-        <v>19.543141302308126</v>
+        <v>19.663538123735307</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -4749,14 +4749,14 @@
         <v>1024</v>
       </c>
       <c r="D54">
-        <v>5.2072700000000003</v>
+        <v>4.5672499999999996</v>
       </c>
       <c r="E54">
-        <v>0.30264000000000002</v>
+        <v>0.28586</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" si="6"/>
-        <v>17.206152524451493</v>
+        <v>15.977226614426641</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -4773,14 +4773,14 @@
         <v>32</v>
       </c>
       <c r="D56">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E56">
-        <v>0.59197</v>
+        <v>0.57065999999999995</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" ref="F56:F61" si="7">D56/E56</f>
-        <v>20.660844299542209</v>
+        <v>18.504486033715349</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -4794,14 +4794,14 @@
         <v>64</v>
       </c>
       <c r="D57">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E57">
-        <v>0.55881999999999998</v>
+        <v>0.48305999999999999</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" si="7"/>
-        <v>21.886475072474145</v>
+        <v>21.860162298679253</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -4815,14 +4815,14 @@
         <v>128</v>
       </c>
       <c r="D58">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E58">
-        <v>0.53861000000000003</v>
+        <v>0.45971000000000001</v>
       </c>
       <c r="F58" s="2">
         <f t="shared" si="7"/>
-        <v>22.70771058836635</v>
+        <v>22.970503143285985</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -4836,14 +4836,14 @@
         <v>256</v>
       </c>
       <c r="D59">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E59">
-        <v>0.51846000000000003</v>
+        <v>0.46072999999999997</v>
       </c>
       <c r="F59" s="2">
         <f t="shared" si="7"/>
-        <v>23.590248042279057</v>
+        <v>22.919649252273569</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>7</v>
@@ -4860,14 +4860,14 @@
         <v>512</v>
       </c>
       <c r="D60">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E60">
-        <v>0.53446000000000005</v>
+        <v>0.45900999999999997</v>
       </c>
       <c r="F60" s="2">
         <f t="shared" si="7"/>
-        <v>22.884032481383077</v>
+        <v>23.005533648504393</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -4881,14 +4881,14 @@
         <v>1024</v>
       </c>
       <c r="D61">
-        <v>12.230600000000001</v>
+        <v>10.55977</v>
       </c>
       <c r="E61">
-        <v>0.62161</v>
+        <v>0.55408000000000002</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" si="7"/>
-        <v>19.675680893164525</v>
+        <v>19.058204591394745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>